<commit_message>
Enhance main.py layout and functionality, update progress bar configuration, and add garments_sp_search.py for data retrieval and processing
</commit_message>
<xml_diff>
--- a/color_wise_output.xlsx
+++ b/color_wise_output.xlsx
@@ -8,14 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1. Work\test\Fabric_Followup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D6B86F-FBAE-4D3E-9AC1-02BC4C876667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0F05EC-4B93-4359-878D-A1380500B7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -503,7 +514,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -515,6 +526,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -552,12 +569,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -865,7 +885,7 @@
   <dimension ref="A1:AC59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,7 +983,7 @@
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C2" s="2" t="s">

</xml_diff>